<commit_message>
fixes typos in IRIs, resolves #81; updates terms
The following typos in IRIs were fixed using the new SHACL shapes from
previous commit:
- dpv:expiry relation instead of dpv:hasExpiry relation in consent
- dpv:hasConsequenceOn was used as a parent even though it was proposed.
  The term has been promoted to accepted status
- Typos in Technical measures where Crypto- was mistyped as Cryto-

Errors in labels:
- MaintainCreditCheckingDatabase
- MaintainCreditRatingDatabase

The following terms were updated:
- GDPR's legal bases where text has been added from Art.6 and the parent
  terms have been aligned with main spec's legal bases (including
  creation of new terms to match granularity)
- Anonymisation and Pseudonymisation have been changed to be types of
  Deidentification techniques (as the grouping parent concept) to
  distinguish them following discussions in #15
- DPV-LEGAL has laws and DPAs for USA from contributions by @JonathanBowker
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/location_jurisdiction.xlsx
+++ b/documentation-generator/vocab_csv/location_jurisdiction.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="1557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4174" uniqueCount="1573">
   <si>
     <t>Term</t>
   </si>
@@ -3863,7 +3863,7 @@
     <t>Jonathan Bowker</t>
   </si>
   <si>
-    <t>GB-DPA-2018</t>
+    <t>GB-DPA</t>
   </si>
   <si>
     <t>Data Protection Act (DPA)</t>
@@ -3887,13 +3887,10 @@
     <t>Virginia Consumer Data Protection Act (VCDPA)</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>dpv-legal:US-VA</t>
   </si>
   <si>
-    <t>https://lis.virginia.gov/cgi-bin/legp604.exe?211+sum+SB1392</t>
+    <t>https://lis.virginia.gov/cgi-bin/legp604.exe?212+sum+HB2307</t>
   </si>
   <si>
     <t>US-CO-CPA</t>
@@ -3920,7 +3917,7 @@
     <t>https://www.cga.ct.gov/2022/ACT/PA/PDF/2022PA-00015-R00SB-00006-PA.PDF</t>
   </si>
   <si>
-    <t>NPICICA</t>
+    <t>US-NV-NPICICA</t>
   </si>
   <si>
     <t>Nevada Privacy of Information Collected on the Internet from Consumers Act (NPICICA)</t>
@@ -4524,6 +4521,57 @@
   </si>
   <si>
     <t>https://attorneygeneral.utah.gov/</t>
+  </si>
+  <si>
+    <t>DPA-US-VC</t>
+  </si>
+  <si>
+    <t>Virginia Attorney General</t>
+  </si>
+  <si>
+    <t>dpv-legal:US-VC</t>
+  </si>
+  <si>
+    <t>dpv-legal:US-VA-VCDPA</t>
+  </si>
+  <si>
+    <t>https://www.oag.state.va.us</t>
+  </si>
+  <si>
+    <t>DPA-US-CO</t>
+  </si>
+  <si>
+    <t>Colorado Attorney General</t>
+  </si>
+  <si>
+    <t>dpv-legal:US-CO-CPA</t>
+  </si>
+  <si>
+    <t>https://coag.gov</t>
+  </si>
+  <si>
+    <t>DPA-US-CT</t>
+  </si>
+  <si>
+    <t>Connecticut Attorney General</t>
+  </si>
+  <si>
+    <t>dpv-legal:US-CT-CTPA</t>
+  </si>
+  <si>
+    <t>https://portal.ct.gov/AG</t>
+  </si>
+  <si>
+    <t>DPA-US-NV</t>
+  </si>
+  <si>
+    <t>Nevada Attorney General</t>
+  </si>
+  <si>
+    <t>dpv-legal:US-NV-NPICICA</t>
+  </si>
+  <si>
+    <t>https://ag.nv.gov/</t>
   </si>
   <si>
     <t>has Broader</t>
@@ -5498,6 +5546,7 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="24.38"/>
     <col customWidth="1" min="3" max="3" width="45.25"/>
+    <col customWidth="1" min="4" max="4" width="22.0"/>
     <col customWidth="1" min="5" max="5" width="16.75"/>
     <col customWidth="1" min="6" max="6" width="13.75"/>
     <col customWidth="1" min="7" max="7" width="16.0"/>
@@ -25604,7 +25653,7 @@
     <col customWidth="1" min="1" max="1" width="20.75"/>
     <col customWidth="1" min="2" max="2" width="41.63"/>
     <col customWidth="1" min="6" max="6" width="25.13"/>
-    <col customWidth="1" min="7" max="7" width="32.63"/>
+    <col customWidth="1" min="7" max="7" width="57.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
@@ -26659,7 +26708,7 @@
         <v>1264</v>
       </c>
       <c r="D29" s="12">
-        <v>44704.0</v>
+        <v>43245.0</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>1265</v>
@@ -26722,66 +26771,166 @@
       <c r="B32" s="10" t="s">
         <v>1270</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="12">
+        <v>44927.0</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="10" t="s">
         <v>1271</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="G32" s="32" t="s">
         <v>1272</v>
       </c>
-      <c r="G32" s="32" t="s">
-        <v>1273</v>
-      </c>
+      <c r="H32" s="12">
+        <v>44888.0</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>1274</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="C33" s="11"/>
+      <c r="D33" s="12">
+        <v>45298.0</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="10" t="s">
         <v>1275</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>1271</v>
-      </c>
-      <c r="F33" s="10" t="s">
+      <c r="G33" s="32" t="s">
         <v>1276</v>
       </c>
-      <c r="G33" s="32" t="s">
-        <v>1277</v>
-      </c>
+      <c r="H33" s="19">
+        <v>44888.0</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>1278</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="12">
+        <v>44933.0</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="10" t="s">
         <v>1279</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>1271</v>
-      </c>
-      <c r="F34" s="10" t="s">
+      <c r="G34" s="13" t="s">
         <v>1280</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>1281</v>
-      </c>
+      <c r="H34" s="19">
+        <v>44888.0</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>1282</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="11"/>
+      <c r="D35" s="12">
+        <v>44206.0</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="10" t="s">
         <v>1283</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>1271</v>
-      </c>
-      <c r="F35" s="10" t="s">
+      <c r="G35" s="13" t="s">
         <v>1284</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>1285</v>
-      </c>
+      <c r="H35" s="19">
+        <v>44888.0</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:X174">
@@ -26907,6 +27056,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="2" max="2" width="47.38"/>
     <col customWidth="1" min="4" max="4" width="23.38"/>
     <col customWidth="1" min="5" max="5" width="16.25"/>
     <col customWidth="1" min="6" max="6" width="39.13"/>
@@ -26924,13 +27074,13 @@
         <v>1155</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>1286</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1287</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>1288</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1159</v>
@@ -26953,7 +27103,7 @@
     </row>
     <row r="2">
       <c r="A2" s="40" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="57"/>
@@ -26982,23 +27132,23 @@
     </row>
     <row r="3">
       <c r="A3" s="56" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B3" s="56" t="s">
         <v>1290</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>1291</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="58" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E3" s="56" t="s">
         <v>1292</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="F3" s="56" t="s">
         <v>1293</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="G3" s="61" t="s">
         <v>1294</v>
-      </c>
-      <c r="G3" s="61" t="s">
-        <v>1295</v>
       </c>
       <c r="H3" s="59">
         <v>44650.0</v>
@@ -27029,23 +27179,23 @@
     </row>
     <row r="4">
       <c r="A4" s="56" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B4" s="56" t="s">
         <v>1296</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>1297</v>
       </c>
       <c r="C4" s="57"/>
       <c r="D4" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E4" s="56" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G4" s="61" t="s">
         <v>1298</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G4" s="61" t="s">
-        <v>1299</v>
       </c>
       <c r="H4" s="59">
         <v>44650.0</v>
@@ -27076,23 +27226,23 @@
     </row>
     <row r="5">
       <c r="A5" s="56" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B5" s="56" t="s">
         <v>1300</v>
-      </c>
-      <c r="B5" s="56" t="s">
-        <v>1301</v>
       </c>
       <c r="C5" s="57"/>
       <c r="D5" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E5" s="56" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G5" s="61" t="s">
         <v>1302</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G5" s="61" t="s">
-        <v>1303</v>
       </c>
       <c r="H5" s="59">
         <v>44650.0</v>
@@ -27123,23 +27273,23 @@
     </row>
     <row r="6">
       <c r="A6" s="56" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B6" s="56" t="s">
         <v>1304</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>1305</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E6" s="56" t="s">
+        <v>1305</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G6" s="61" t="s">
         <v>1306</v>
-      </c>
-      <c r="F6" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G6" s="61" t="s">
-        <v>1307</v>
       </c>
       <c r="H6" s="59">
         <v>44650.0</v>
@@ -27170,23 +27320,23 @@
     </row>
     <row r="7">
       <c r="A7" s="56" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B7" s="56" t="s">
         <v>1308</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>1309</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E7" s="56" t="s">
         <v>233</v>
       </c>
       <c r="F7" s="56" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G7" s="61" t="s">
         <v>1310</v>
-      </c>
-      <c r="G7" s="61" t="s">
-        <v>1311</v>
       </c>
       <c r="H7" s="59">
         <v>44650.0</v>
@@ -27217,25 +27367,25 @@
     </row>
     <row r="8">
       <c r="A8" s="56" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B8" s="56" t="s">
         <v>1312</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="C8" s="56" t="s">
         <v>1313</v>
       </c>
-      <c r="C8" s="56" t="s">
-        <v>1314</v>
-      </c>
       <c r="D8" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E8" s="56" t="s">
         <v>1169</v>
       </c>
       <c r="F8" s="56" t="s">
+        <v>1314</v>
+      </c>
+      <c r="G8" s="61" t="s">
         <v>1315</v>
-      </c>
-      <c r="G8" s="61" t="s">
-        <v>1316</v>
       </c>
       <c r="H8" s="59">
         <v>44650.0</v>
@@ -27266,25 +27416,25 @@
     </row>
     <row r="9">
       <c r="A9" s="56" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>1317</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="C9" s="56" t="s">
         <v>1318</v>
       </c>
-      <c r="C9" s="56" t="s">
-        <v>1319</v>
-      </c>
       <c r="D9" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E9" s="56" t="s">
         <v>1174</v>
       </c>
       <c r="F9" s="56" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G9" s="61" t="s">
         <v>1320</v>
-      </c>
-      <c r="G9" s="61" t="s">
-        <v>1321</v>
       </c>
       <c r="H9" s="59">
         <v>44650.0</v>
@@ -27315,25 +27465,25 @@
     </row>
     <row r="10">
       <c r="A10" s="56" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B10" s="56" t="s">
         <v>1322</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="C10" s="56" t="s">
         <v>1323</v>
       </c>
-      <c r="C10" s="56" t="s">
-        <v>1324</v>
-      </c>
       <c r="D10" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E10" s="56" t="s">
         <v>1184</v>
       </c>
       <c r="F10" s="56" t="s">
+        <v>1324</v>
+      </c>
+      <c r="G10" s="61" t="s">
         <v>1325</v>
-      </c>
-      <c r="G10" s="61" t="s">
-        <v>1326</v>
       </c>
       <c r="H10" s="59">
         <v>44650.0</v>
@@ -27364,25 +27514,25 @@
     </row>
     <row r="11">
       <c r="A11" s="56" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B11" s="56" t="s">
         <v>1327</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="C11" s="56" t="s">
         <v>1328</v>
       </c>
-      <c r="C11" s="56" t="s">
-        <v>1329</v>
-      </c>
       <c r="D11" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E11" s="56" t="s">
         <v>1184</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="H11" s="59">
         <v>44650.0</v>
@@ -27413,25 +27563,25 @@
     </row>
     <row r="12">
       <c r="A12" s="56" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B12" s="56" t="s">
         <v>1331</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="C12" s="56" t="s">
         <v>1332</v>
       </c>
-      <c r="C12" s="56" t="s">
-        <v>1333</v>
-      </c>
       <c r="D12" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E12" s="56" t="s">
         <v>1189</v>
       </c>
       <c r="F12" s="56" t="s">
+        <v>1333</v>
+      </c>
+      <c r="G12" s="61" t="s">
         <v>1334</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>1335</v>
       </c>
       <c r="H12" s="59">
         <v>44650.0</v>
@@ -27462,25 +27612,25 @@
     </row>
     <row r="13">
       <c r="A13" s="56" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B13" s="56" t="s">
         <v>1336</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="C13" s="56" t="s">
         <v>1337</v>
       </c>
-      <c r="C13" s="56" t="s">
-        <v>1338</v>
-      </c>
       <c r="D13" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E13" s="56" t="s">
         <v>1194</v>
       </c>
       <c r="F13" s="56" t="s">
+        <v>1338</v>
+      </c>
+      <c r="G13" s="61" t="s">
         <v>1339</v>
-      </c>
-      <c r="G13" s="61" t="s">
-        <v>1340</v>
       </c>
       <c r="H13" s="59">
         <v>44650.0</v>
@@ -27511,25 +27661,25 @@
     </row>
     <row r="14">
       <c r="A14" s="56" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B14" s="56" t="s">
         <v>1341</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="C14" s="56" t="s">
         <v>1342</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>1343</v>
-      </c>
       <c r="D14" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E14" s="56" t="s">
         <v>1199</v>
       </c>
       <c r="F14" s="56" t="s">
+        <v>1343</v>
+      </c>
+      <c r="G14" s="61" t="s">
         <v>1344</v>
-      </c>
-      <c r="G14" s="61" t="s">
-        <v>1345</v>
       </c>
       <c r="H14" s="59">
         <v>44650.0</v>
@@ -27560,25 +27710,25 @@
     </row>
     <row r="15">
       <c r="A15" s="56" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B15" s="56" t="s">
         <v>1346</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="C15" s="56" t="s">
         <v>1347</v>
       </c>
-      <c r="C15" s="56" t="s">
-        <v>1348</v>
-      </c>
       <c r="D15" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E15" s="56" t="s">
         <v>1209</v>
       </c>
       <c r="F15" s="56" t="s">
+        <v>1348</v>
+      </c>
+      <c r="G15" s="61" t="s">
         <v>1349</v>
-      </c>
-      <c r="G15" s="61" t="s">
-        <v>1350</v>
       </c>
       <c r="H15" s="59">
         <v>44650.0</v>
@@ -27609,25 +27759,25 @@
     </row>
     <row r="16">
       <c r="A16" s="56" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B16" s="56" t="s">
         <v>1351</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="C16" s="56" t="s">
         <v>1352</v>
       </c>
-      <c r="C16" s="56" t="s">
-        <v>1353</v>
-      </c>
       <c r="D16" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>1214</v>
       </c>
       <c r="F16" s="56" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G16" s="61" t="s">
         <v>1354</v>
-      </c>
-      <c r="G16" s="61" t="s">
-        <v>1355</v>
       </c>
       <c r="H16" s="59">
         <v>44650.0</v>
@@ -27658,25 +27808,25 @@
     </row>
     <row r="17">
       <c r="A17" s="56" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B17" s="56" t="s">
         <v>1356</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="C17" s="56" t="s">
         <v>1357</v>
       </c>
-      <c r="C17" s="56" t="s">
-        <v>1358</v>
-      </c>
       <c r="D17" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E17" s="56" t="s">
         <v>1219</v>
       </c>
       <c r="F17" s="56" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G17" s="61" t="s">
         <v>1359</v>
-      </c>
-      <c r="G17" s="61" t="s">
-        <v>1360</v>
       </c>
       <c r="H17" s="59">
         <v>44650.0</v>
@@ -27707,25 +27857,25 @@
     </row>
     <row r="18">
       <c r="A18" s="56" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B18" s="56" t="s">
         <v>1361</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="C18" s="56" t="s">
         <v>1362</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="D18" s="58" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E18" s="56" t="s">
         <v>1363</v>
       </c>
-      <c r="D18" s="58" t="s">
-        <v>1292</v>
-      </c>
-      <c r="E18" s="56" t="s">
+      <c r="F18" s="56" t="s">
         <v>1364</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="G18" s="61" t="s">
         <v>1365</v>
-      </c>
-      <c r="G18" s="61" t="s">
-        <v>1366</v>
       </c>
       <c r="H18" s="59">
         <v>44650.0</v>
@@ -27756,25 +27906,25 @@
     </row>
     <row r="19">
       <c r="A19" s="56" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B19" s="56" t="s">
         <v>1367</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="C19" s="56" t="s">
         <v>1368</v>
       </c>
-      <c r="C19" s="56" t="s">
-        <v>1369</v>
-      </c>
       <c r="D19" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E19" s="56" t="s">
         <v>1229</v>
       </c>
       <c r="F19" s="56" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G19" s="61" t="s">
         <v>1370</v>
-      </c>
-      <c r="G19" s="61" t="s">
-        <v>1371</v>
       </c>
       <c r="H19" s="59">
         <v>44650.0</v>
@@ -27805,25 +27955,25 @@
     </row>
     <row r="20">
       <c r="A20" s="56" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B20" s="56" t="s">
         <v>1372</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="C20" s="56" t="s">
         <v>1373</v>
       </c>
-      <c r="C20" s="56" t="s">
-        <v>1374</v>
-      </c>
       <c r="D20" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E20" s="56" t="s">
         <v>1234</v>
       </c>
       <c r="F20" s="56" t="s">
+        <v>1374</v>
+      </c>
+      <c r="G20" s="61" t="s">
         <v>1375</v>
-      </c>
-      <c r="G20" s="61" t="s">
-        <v>1376</v>
       </c>
       <c r="H20" s="59">
         <v>44650.0</v>
@@ -27854,25 +28004,25 @@
     </row>
     <row r="21">
       <c r="A21" s="56" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B21" s="56" t="s">
         <v>1377</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="C21" s="56" t="s">
         <v>1378</v>
       </c>
-      <c r="C21" s="56" t="s">
-        <v>1379</v>
-      </c>
       <c r="D21" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E21" s="56" t="s">
         <v>1239</v>
       </c>
       <c r="F21" s="56" t="s">
+        <v>1379</v>
+      </c>
+      <c r="G21" s="61" t="s">
         <v>1380</v>
-      </c>
-      <c r="G21" s="61" t="s">
-        <v>1381</v>
       </c>
       <c r="H21" s="59">
         <v>44650.0</v>
@@ -27903,25 +28053,25 @@
     </row>
     <row r="22">
       <c r="A22" s="56" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B22" s="56" t="s">
         <v>1382</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="C22" s="56" t="s">
         <v>1383</v>
       </c>
-      <c r="C22" s="56" t="s">
-        <v>1384</v>
-      </c>
       <c r="D22" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E22" s="56" t="s">
         <v>1204</v>
       </c>
       <c r="F22" s="56" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G22" s="61" t="s">
         <v>1385</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>1386</v>
       </c>
       <c r="H22" s="59">
         <v>44650.0</v>
@@ -27952,25 +28102,25 @@
     </row>
     <row r="23">
       <c r="A23" s="56" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B23" s="56" t="s">
         <v>1387</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="C23" s="56" t="s">
         <v>1388</v>
       </c>
-      <c r="C23" s="56" t="s">
-        <v>1389</v>
-      </c>
       <c r="D23" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E23" s="56" t="s">
         <v>1244</v>
       </c>
       <c r="F23" s="56" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G23" s="61" t="s">
         <v>1390</v>
-      </c>
-      <c r="G23" s="61" t="s">
-        <v>1391</v>
       </c>
       <c r="H23" s="59">
         <v>44650.0</v>
@@ -28001,23 +28151,23 @@
     </row>
     <row r="24">
       <c r="A24" s="56" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B24" s="56" t="s">
         <v>1392</v>
-      </c>
-      <c r="B24" s="56" t="s">
-        <v>1393</v>
       </c>
       <c r="C24" s="63"/>
       <c r="D24" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E24" s="56" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F24" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G24" s="61" t="s">
         <v>1394</v>
-      </c>
-      <c r="F24" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G24" s="61" t="s">
-        <v>1395</v>
       </c>
       <c r="H24" s="59">
         <v>44650.0</v>
@@ -28048,23 +28198,23 @@
     </row>
     <row r="25">
       <c r="A25" s="56" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B25" s="56" t="s">
         <v>1396</v>
-      </c>
-      <c r="B25" s="56" t="s">
-        <v>1397</v>
       </c>
       <c r="C25" s="63"/>
       <c r="D25" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E25" s="56" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F25" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G25" s="61" t="s">
         <v>1398</v>
-      </c>
-      <c r="F25" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G25" s="61" t="s">
-        <v>1399</v>
       </c>
       <c r="H25" s="59">
         <v>44650.0</v>
@@ -28095,23 +28245,23 @@
     </row>
     <row r="26">
       <c r="A26" s="56" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B26" s="56" t="s">
         <v>1400</v>
-      </c>
-      <c r="B26" s="56" t="s">
-        <v>1401</v>
       </c>
       <c r="C26" s="63"/>
       <c r="D26" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E26" s="56" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F26" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G26" s="61" t="s">
         <v>1402</v>
-      </c>
-      <c r="F26" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G26" s="61" t="s">
-        <v>1403</v>
       </c>
       <c r="H26" s="59">
         <v>44650.0</v>
@@ -28142,23 +28292,23 @@
     </row>
     <row r="27">
       <c r="A27" s="56" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B27" s="56" t="s">
         <v>1404</v>
-      </c>
-      <c r="B27" s="56" t="s">
-        <v>1405</v>
       </c>
       <c r="C27" s="63"/>
       <c r="D27" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E27" s="56" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G27" s="61" t="s">
         <v>1406</v>
-      </c>
-      <c r="F27" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G27" s="61" t="s">
-        <v>1407</v>
       </c>
       <c r="H27" s="59">
         <v>44650.0</v>
@@ -28189,23 +28339,23 @@
     </row>
     <row r="28">
       <c r="A28" s="56" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B28" s="56" t="s">
         <v>1408</v>
-      </c>
-      <c r="B28" s="56" t="s">
-        <v>1409</v>
       </c>
       <c r="C28" s="63"/>
       <c r="D28" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E28" s="56" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F28" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G28" s="61" t="s">
         <v>1410</v>
-      </c>
-      <c r="F28" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G28" s="61" t="s">
-        <v>1411</v>
       </c>
       <c r="H28" s="59">
         <v>44650.0</v>
@@ -28236,23 +28386,23 @@
     </row>
     <row r="29">
       <c r="A29" s="56" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B29" s="56" t="s">
         <v>1412</v>
-      </c>
-      <c r="B29" s="56" t="s">
-        <v>1413</v>
       </c>
       <c r="C29" s="63"/>
       <c r="D29" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E29" s="56" t="s">
+        <v>1413</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G29" s="61" t="s">
         <v>1414</v>
-      </c>
-      <c r="F29" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G29" s="61" t="s">
-        <v>1415</v>
       </c>
       <c r="H29" s="59">
         <v>44650.0</v>
@@ -28283,23 +28433,23 @@
     </row>
     <row r="30">
       <c r="A30" s="56" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B30" s="56" t="s">
         <v>1416</v>
-      </c>
-      <c r="B30" s="56" t="s">
-        <v>1417</v>
       </c>
       <c r="C30" s="63"/>
       <c r="D30" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E30" s="56" t="s">
+        <v>1417</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G30" s="61" t="s">
         <v>1418</v>
-      </c>
-      <c r="F30" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G30" s="61" t="s">
-        <v>1419</v>
       </c>
       <c r="H30" s="59">
         <v>44650.0</v>
@@ -28330,23 +28480,23 @@
     </row>
     <row r="31">
       <c r="A31" s="56" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B31" s="56" t="s">
         <v>1420</v>
-      </c>
-      <c r="B31" s="56" t="s">
-        <v>1421</v>
       </c>
       <c r="C31" s="63"/>
       <c r="D31" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E31" s="56" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G31" s="61" t="s">
         <v>1422</v>
-      </c>
-      <c r="F31" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G31" s="61" t="s">
-        <v>1423</v>
       </c>
       <c r="H31" s="59">
         <v>44650.0</v>
@@ -28377,23 +28527,23 @@
     </row>
     <row r="32">
       <c r="A32" s="56" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B32" s="56" t="s">
         <v>1424</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>1425</v>
       </c>
       <c r="C32" s="63"/>
       <c r="D32" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E32" s="56" t="s">
+        <v>1425</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G32" s="61" t="s">
         <v>1426</v>
-      </c>
-      <c r="F32" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G32" s="61" t="s">
-        <v>1427</v>
       </c>
       <c r="H32" s="59">
         <v>44650.0</v>
@@ -28424,23 +28574,23 @@
     </row>
     <row r="33">
       <c r="A33" s="56" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B33" s="56" t="s">
         <v>1428</v>
-      </c>
-      <c r="B33" s="56" t="s">
-        <v>1429</v>
       </c>
       <c r="C33" s="63"/>
       <c r="D33" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E33" s="56" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F33" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G33" s="61" t="s">
         <v>1430</v>
-      </c>
-      <c r="F33" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G33" s="61" t="s">
-        <v>1431</v>
       </c>
       <c r="H33" s="59">
         <v>44650.0</v>
@@ -28471,23 +28621,23 @@
     </row>
     <row r="34">
       <c r="A34" s="56" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B34" s="56" t="s">
         <v>1432</v>
-      </c>
-      <c r="B34" s="56" t="s">
-        <v>1433</v>
       </c>
       <c r="C34" s="63"/>
       <c r="D34" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E34" s="56" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F34" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G34" s="61" t="s">
         <v>1434</v>
-      </c>
-      <c r="F34" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G34" s="61" t="s">
-        <v>1435</v>
       </c>
       <c r="H34" s="59">
         <v>44650.0</v>
@@ -28518,23 +28668,23 @@
     </row>
     <row r="35">
       <c r="A35" s="56" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B35" s="56" t="s">
         <v>1436</v>
-      </c>
-      <c r="B35" s="56" t="s">
-        <v>1437</v>
       </c>
       <c r="C35" s="63"/>
       <c r="D35" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E35" s="56" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F35" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G35" s="61" t="s">
         <v>1438</v>
-      </c>
-      <c r="F35" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G35" s="61" t="s">
-        <v>1439</v>
       </c>
       <c r="H35" s="59">
         <v>44650.0</v>
@@ -28565,23 +28715,23 @@
     </row>
     <row r="36">
       <c r="A36" s="56" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B36" s="56" t="s">
         <v>1440</v>
-      </c>
-      <c r="B36" s="56" t="s">
-        <v>1441</v>
       </c>
       <c r="C36" s="63"/>
       <c r="D36" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E36" s="56" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F36" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G36" s="61" t="s">
         <v>1442</v>
-      </c>
-      <c r="F36" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G36" s="61" t="s">
-        <v>1443</v>
       </c>
       <c r="H36" s="59">
         <v>44650.0</v>
@@ -28612,23 +28762,23 @@
     </row>
     <row r="37">
       <c r="A37" s="56" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B37" s="56" t="s">
         <v>1444</v>
-      </c>
-      <c r="B37" s="56" t="s">
-        <v>1445</v>
       </c>
       <c r="C37" s="63"/>
       <c r="D37" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E37" s="56" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F37" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G37" s="61" t="s">
         <v>1446</v>
-      </c>
-      <c r="F37" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G37" s="61" t="s">
-        <v>1447</v>
       </c>
       <c r="H37" s="59">
         <v>44650.0</v>
@@ -28659,23 +28809,23 @@
     </row>
     <row r="38">
       <c r="A38" s="56" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B38" s="58" t="s">
         <v>1448</v>
-      </c>
-      <c r="B38" s="58" t="s">
-        <v>1449</v>
       </c>
       <c r="C38" s="63"/>
       <c r="D38" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E38" s="56" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F38" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G38" s="61" t="s">
         <v>1450</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G38" s="61" t="s">
-        <v>1451</v>
       </c>
       <c r="H38" s="59">
         <v>44650.0</v>
@@ -28706,23 +28856,23 @@
     </row>
     <row r="39">
       <c r="A39" s="56" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B39" s="56" t="s">
         <v>1452</v>
-      </c>
-      <c r="B39" s="56" t="s">
-        <v>1453</v>
       </c>
       <c r="C39" s="63"/>
       <c r="D39" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E39" s="56" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F39" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G39" s="61" t="s">
         <v>1454</v>
-      </c>
-      <c r="F39" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G39" s="61" t="s">
-        <v>1455</v>
       </c>
       <c r="H39" s="59">
         <v>44650.0</v>
@@ -28753,23 +28903,23 @@
     </row>
     <row r="40">
       <c r="A40" s="56" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B40" s="56" t="s">
         <v>1456</v>
-      </c>
-      <c r="B40" s="56" t="s">
-        <v>1457</v>
       </c>
       <c r="C40" s="63"/>
       <c r="D40" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E40" s="56" t="s">
+        <v>1457</v>
+      </c>
+      <c r="F40" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G40" s="61" t="s">
         <v>1458</v>
-      </c>
-      <c r="F40" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G40" s="61" t="s">
-        <v>1459</v>
       </c>
       <c r="H40" s="59">
         <v>44650.0</v>
@@ -28800,23 +28950,23 @@
     </row>
     <row r="41">
       <c r="A41" s="56" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B41" s="56" t="s">
         <v>1460</v>
-      </c>
-      <c r="B41" s="56" t="s">
-        <v>1461</v>
       </c>
       <c r="C41" s="63"/>
       <c r="D41" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E41" s="56" t="s">
+        <v>1461</v>
+      </c>
+      <c r="F41" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G41" s="61" t="s">
         <v>1462</v>
-      </c>
-      <c r="F41" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G41" s="61" t="s">
-        <v>1463</v>
       </c>
       <c r="H41" s="59">
         <v>44650.0</v>
@@ -28847,23 +28997,23 @@
     </row>
     <row r="42">
       <c r="A42" s="56" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B42" s="56" t="s">
         <v>1464</v>
-      </c>
-      <c r="B42" s="56" t="s">
-        <v>1465</v>
       </c>
       <c r="C42" s="63"/>
       <c r="D42" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E42" s="56" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F42" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G42" s="61" t="s">
         <v>1466</v>
-      </c>
-      <c r="F42" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G42" s="61" t="s">
-        <v>1467</v>
       </c>
       <c r="H42" s="59">
         <v>44650.0</v>
@@ -28894,23 +29044,23 @@
     </row>
     <row r="43">
       <c r="A43" s="56" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B43" s="56" t="s">
         <v>1468</v>
-      </c>
-      <c r="B43" s="56" t="s">
-        <v>1469</v>
       </c>
       <c r="C43" s="63"/>
       <c r="D43" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E43" s="56" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F43" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G43" s="61" t="s">
         <v>1470</v>
-      </c>
-      <c r="F43" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G43" s="61" t="s">
-        <v>1471</v>
       </c>
       <c r="H43" s="59">
         <v>44650.0</v>
@@ -28941,23 +29091,23 @@
     </row>
     <row r="44">
       <c r="A44" s="56" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B44" s="56" t="s">
         <v>1472</v>
-      </c>
-      <c r="B44" s="56" t="s">
-        <v>1473</v>
       </c>
       <c r="C44" s="63"/>
       <c r="D44" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E44" s="56" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F44" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G44" s="61" t="s">
         <v>1474</v>
-      </c>
-      <c r="F44" s="56" t="s">
-        <v>1294</v>
-      </c>
-      <c r="G44" s="61" t="s">
-        <v>1475</v>
       </c>
       <c r="H44" s="59">
         <v>44650.0</v>
@@ -28988,23 +29138,23 @@
     </row>
     <row r="45">
       <c r="A45" s="60" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B45" s="60" t="s">
         <v>1476</v>
-      </c>
-      <c r="B45" s="60" t="s">
-        <v>1477</v>
       </c>
       <c r="C45" s="44"/>
       <c r="D45" s="58" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E45" s="60" t="s">
         <v>1265</v>
       </c>
       <c r="F45" s="58" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G45" s="62" t="s">
         <v>1478</v>
-      </c>
-      <c r="G45" s="62" t="s">
-        <v>1479</v>
       </c>
       <c r="H45" s="59">
         <v>44762.0</v>
@@ -29035,23 +29185,23 @@
     </row>
     <row r="46">
       <c r="A46" s="10" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>1480</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>1481</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="64" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>1260</v>
       </c>
       <c r="F46" s="10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="G46" s="13" t="s">
         <v>1482</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>1483</v>
       </c>
       <c r="H46" s="12">
         <v>44887.0</v>
@@ -29076,6 +29226,182 @@
       <c r="V46" s="11"/>
       <c r="W46" s="11"/>
       <c r="X46" s="11"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="10" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="64" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>1486</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="H47" s="12">
+        <v>44888.0</v>
+      </c>
+      <c r="I47" s="11"/>
+      <c r="J47" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="10" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="64" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H48" s="12">
+        <v>44888.0</v>
+      </c>
+      <c r="I48" s="11"/>
+      <c r="J48" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="64" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>1495</v>
+      </c>
+      <c r="H49" s="12">
+        <v>44888.0</v>
+      </c>
+      <c r="I49" s="11"/>
+      <c r="J49" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="10" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="10" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>1498</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H50" s="12">
+        <v>44888.0</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:X168">
@@ -29181,8 +29507,12 @@
     <hyperlink r:id="rId85" ref="G45"/>
     <hyperlink r:id="rId86" ref="L45"/>
     <hyperlink r:id="rId87" ref="G46"/>
+    <hyperlink r:id="rId88" ref="G47"/>
+    <hyperlink r:id="rId89" ref="G48"/>
+    <hyperlink r:id="rId90" ref="G49"/>
+    <hyperlink r:id="rId91" ref="G50"/>
   </hyperlinks>
-  <drawing r:id="rId88"/>
+  <drawing r:id="rId92"/>
 </worksheet>
 </file>
 
@@ -29200,6 +29530,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="2" max="2" width="33.38"/>
+    <col customWidth="1" min="3" max="3" width="25.25"/>
+    <col customWidth="1" min="11" max="11" width="27.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
@@ -29213,16 +29546,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1484</v>
+        <v>1500</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1485</v>
+        <v>1501</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1486</v>
+        <v>1502</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>1487</v>
+        <v>1503</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>10</v>
@@ -29242,19 +29575,19 @@
     </row>
     <row r="2">
       <c r="A2" s="45" t="s">
-        <v>1488</v>
+        <v>1504</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>1489</v>
+        <v>1505</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>1490</v>
+        <v>1506</v>
       </c>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
       <c r="G2" s="66" t="s">
-        <v>1491</v>
+        <v>1507</v>
       </c>
       <c r="H2" s="19">
         <v>44650.0</v>
@@ -29284,23 +29617,23 @@
     </row>
     <row r="3">
       <c r="A3" s="45" t="s">
-        <v>1492</v>
+        <v>1508</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>1493</v>
+        <v>1509</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>1490</v>
+        <v>1506</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>1494</v>
+        <v>1510</v>
       </c>
       <c r="E3" s="50">
         <v>43862.0</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="45" t="s">
-        <v>1491</v>
+        <v>1507</v>
       </c>
       <c r="H3" s="19">
         <v>44650.0</v>
@@ -29330,16 +29663,16 @@
     </row>
     <row r="4">
       <c r="A4" s="45" t="s">
-        <v>1495</v>
+        <v>1511</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>1496</v>
+        <v>1512</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>1490</v>
+        <v>1506</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>1494</v>
+        <v>1510</v>
       </c>
       <c r="E4" s="50">
         <v>41741.0</v>
@@ -29348,7 +29681,7 @@
         <v>43861.0</v>
       </c>
       <c r="G4" s="45" t="s">
-        <v>1497</v>
+        <v>1513</v>
       </c>
       <c r="H4" s="19">
         <v>44650.0</v>
@@ -29381,16 +29714,16 @@
         <v>1246</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>1498</v>
+        <v>1514</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>1490</v>
+        <v>1506</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="45" t="s">
-        <v>1491</v>
+        <v>1507</v>
       </c>
       <c r="H5" s="19">
         <v>44650.0</v>
@@ -29420,23 +29753,23 @@
     </row>
     <row r="6">
       <c r="A6" s="45" t="s">
-        <v>1499</v>
+        <v>1515</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>1500</v>
+        <v>1516</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>1490</v>
+        <v>1506</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E6" s="50">
         <v>43862.0</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="45" t="s">
-        <v>1491</v>
+        <v>1507</v>
       </c>
       <c r="H6" s="19">
         <v>44650.0</v>
@@ -29466,16 +29799,16 @@
     </row>
     <row r="7">
       <c r="A7" s="45" t="s">
-        <v>1502</v>
+        <v>1518</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>1503</v>
+        <v>1519</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>1490</v>
+        <v>1506</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E7" s="50">
         <v>41456.0</v>
@@ -29484,7 +29817,7 @@
         <v>43861.0</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>1497</v>
+        <v>1513</v>
       </c>
       <c r="H7" s="19">
         <v>44650.0</v>
@@ -33037,16 +33370,16 @@
         <v>1159</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1504</v>
+        <v>1520</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1505</v>
+        <v>1521</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1485</v>
+        <v>1501</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>1486</v>
+        <v>1502</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>10</v>
@@ -33066,19 +33399,19 @@
     </row>
     <row r="2">
       <c r="A2" s="45" t="s">
-        <v>1506</v>
+        <v>1522</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>1507</v>
+        <v>1523</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>1508</v>
+        <v>1524</v>
       </c>
       <c r="D2" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>1509</v>
+        <v>1525</v>
       </c>
       <c r="F2" s="50">
         <v>40472.0</v>
@@ -33112,19 +33445,19 @@
     </row>
     <row r="3">
       <c r="A3" s="45" t="s">
-        <v>1510</v>
+        <v>1526</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>1511</v>
+        <v>1527</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>1512</v>
+        <v>1528</v>
       </c>
       <c r="D3" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>1513</v>
+        <v>1529</v>
       </c>
       <c r="F3" s="50">
         <v>37807.0</v>
@@ -33158,19 +33491,19 @@
     </row>
     <row r="4">
       <c r="A4" s="45" t="s">
-        <v>1514</v>
+        <v>1530</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>1515</v>
+        <v>1531</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>1516</v>
+        <v>1532</v>
       </c>
       <c r="D4" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>1517</v>
+        <v>1533</v>
       </c>
       <c r="F4" s="50">
         <v>37260.0</v>
@@ -33204,19 +33537,19 @@
     </row>
     <row r="5">
       <c r="A5" s="45" t="s">
-        <v>1518</v>
+        <v>1534</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>1519</v>
+        <v>1535</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>1520</v>
+        <v>1536</v>
       </c>
       <c r="D5" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>1521</v>
+        <v>1537</v>
       </c>
       <c r="F5" s="50">
         <v>36763.0</v>
@@ -33250,19 +33583,19 @@
     </row>
     <row r="6">
       <c r="A6" s="45" t="s">
-        <v>1522</v>
+        <v>1538</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>1523</v>
+        <v>1539</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>1524</v>
+        <v>1540</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>1525</v>
+        <v>1541</v>
       </c>
       <c r="F6" s="50">
         <v>40246.0</v>
@@ -33296,16 +33629,16 @@
     </row>
     <row r="7">
       <c r="A7" s="45" t="s">
-        <v>1526</v>
+        <v>1542</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>1527</v>
+        <v>1543</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>1528</v>
+        <v>1544</v>
       </c>
       <c r="D7" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E7" s="45" t="s">
         <v>1265</v>
@@ -33342,19 +33675,19 @@
     </row>
     <row r="8">
       <c r="A8" s="45" t="s">
-        <v>1529</v>
+        <v>1545</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>1530</v>
+        <v>1546</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>1531</v>
+        <v>1547</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>1532</v>
+        <v>1548</v>
       </c>
       <c r="F8" s="50">
         <v>37946.0</v>
@@ -33388,19 +33721,19 @@
     </row>
     <row r="9">
       <c r="A9" s="45" t="s">
-        <v>1533</v>
+        <v>1549</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>1534</v>
+        <v>1550</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>1535</v>
+        <v>1551</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>1536</v>
+        <v>1552</v>
       </c>
       <c r="F9" s="50">
         <v>40575.0</v>
@@ -33434,19 +33767,19 @@
     </row>
     <row r="10">
       <c r="A10" s="45" t="s">
-        <v>1537</v>
+        <v>1553</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>1538</v>
+        <v>1554</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>1539</v>
+        <v>1555</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>1540</v>
+        <v>1556</v>
       </c>
       <c r="F10" s="50">
         <v>38107.0</v>
@@ -33480,19 +33813,19 @@
     </row>
     <row r="11">
       <c r="A11" s="45" t="s">
-        <v>1541</v>
+        <v>1557</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>1542</v>
+        <v>1558</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>1543</v>
+        <v>1559</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>1544</v>
+        <v>1560</v>
       </c>
       <c r="F11" s="50">
         <v>39594.0</v>
@@ -33526,19 +33859,19 @@
     </row>
     <row r="12">
       <c r="A12" s="45" t="s">
-        <v>1545</v>
+        <v>1561</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>1546</v>
+        <v>1562</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>1547</v>
+        <v>1563</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>1548</v>
+        <v>1564</v>
       </c>
       <c r="F12" s="50">
         <v>43488.0</v>
@@ -33572,19 +33905,19 @@
     </row>
     <row r="13">
       <c r="A13" s="45" t="s">
-        <v>1549</v>
+        <v>1565</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>1550</v>
+        <v>1566</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>1551</v>
+        <v>1567</v>
       </c>
       <c r="D13" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>1552</v>
+        <v>1568</v>
       </c>
       <c r="F13" s="50">
         <v>41263.0</v>
@@ -33618,19 +33951,19 @@
     </row>
     <row r="14">
       <c r="A14" s="45" t="s">
-        <v>1553</v>
+        <v>1569</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>1554</v>
+        <v>1570</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>1555</v>
+        <v>1571</v>
       </c>
       <c r="D14" s="66" t="s">
-        <v>1501</v>
+        <v>1517</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>1556</v>
+        <v>1572</v>
       </c>
       <c r="F14" s="50">
         <v>41143.0</v>

</xml_diff>